<commit_message>
Updated Record of work
</commit_message>
<xml_diff>
--- a/doc/KU4 - Record of Work.xlsx
+++ b/doc/KU4 - Record of Work.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeremy\Documents\JeremyBrincat2ndYearProject\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBD4346-0D4C-49CC-8665-2C7A4EC8FEE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2D97B2-5C5E-4425-A5AD-5964BDD8FB99}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43DE01C0-A2D8-4F36-9ADC-E22CC990D539}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43DE01C0-A2D8-4F36-9ADC-E22CC990D539}"/>
   </bookViews>
   <sheets>
     <sheet name="Actual" sheetId="2" r:id="rId1"/>
@@ -1001,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A62287C0-7FD6-48A5-9514-03B257F96545}">
   <dimension ref="A1:R48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1555,9 +1555,9 @@
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -1702,7 +1702,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="29"/>
-      <c r="H32" s="1"/>
+      <c r="H32" s="29"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -1723,8 +1723,8 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
@@ -1745,9 +1745,9 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
@@ -2053,18 +2053,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2200,18 +2200,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FE2ED85-0D3A-4C52-A0D1-D82ED15E39CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D92219-BA5C-4674-AF14-9AA0F4435448}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D92219-BA5C-4674-AF14-9AA0F4435448}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FE2ED85-0D3A-4C52-A0D1-D82ED15E39CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update of Record of Work
</commit_message>
<xml_diff>
--- a/doc/KU4 - Record of Work.xlsx
+++ b/doc/KU4 - Record of Work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeremy\Documents\JeremyBrincat2ndYearProject\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2D97B2-5C5E-4425-A5AD-5964BDD8FB99}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01ACD26A-3EB3-4B10-BFA3-2647F8342FFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43DE01C0-A2D8-4F36-9ADC-E22CC990D539}"/>
   </bookViews>
@@ -1001,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A62287C0-7FD6-48A5-9514-03B257F96545}">
   <dimension ref="A1:R48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,7 +1289,7 @@
       <c r="G12" s="27"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="J12" s="27"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -1558,8 +1558,8 @@
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -1576,11 +1576,11 @@
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -1725,7 +1725,7 @@
       <c r="G33" s="1"/>
       <c r="H33" s="29"/>
       <c r="I33" s="29"/>
-      <c r="J33" s="1"/>
+      <c r="J33" s="29"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -1747,7 +1747,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="29"/>
       <c r="J34" s="29"/>
-      <c r="K34" s="29"/>
+      <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
@@ -2053,18 +2053,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2200,18 +2200,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D92219-BA5C-4674-AF14-9AA0F4435448}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FE2ED85-0D3A-4C52-A0D1-D82ED15E39CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FE2ED85-0D3A-4C52-A0D1-D82ED15E39CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D92219-BA5C-4674-AF14-9AA0F4435448}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>